<commit_message>
saved with cursor at top left cell; opens better
</commit_message>
<xml_diff>
--- a/input/fac_dat_Schools_true_rel.xlsx
+++ b/input/fac_dat_Schools_true_rel.xlsx
@@ -140,6 +140,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -250,10 +251,10 @@
   </sheetPr>
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ALS1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6558" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="ALS1" activeCellId="0" sqref="ALS1"/>
-      <selection pane="bottomLeft" activeCell="ALZ6566" activeCellId="0" sqref="ALZ6566"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -267,11 +268,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1002" min="20" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1003" min="1003" style="2" width="11.52"/>
@@ -1013,7 +1014,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>

</xml_diff>